<commit_message>
Upload the code should move to new direction 2
</commit_message>
<xml_diff>
--- a/Pythons/statistic/Ethics/files/ETHICS.xlsx
+++ b/Pythons/statistic/Ethics/files/ETHICS.xlsx
@@ -69,7 +69,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,12 +87,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -124,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -136,9 +130,6 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -455,15 +446,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -511,16 +502,16 @@
       <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -540,16 +531,16 @@
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -737,7 +728,7 @@
       <c r="C10" s="4">
         <v>10</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -853,7 +844,7 @@
       <c r="C14" s="4">
         <v>35</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -882,7 +873,7 @@
       <c r="C15" s="4">
         <v>25</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -940,22 +931,22 @@
       <c r="C17" s="4">
         <v>25</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="5" t="s">
+      <c r="F17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -969,22 +960,22 @@
       <c r="C18" s="4">
         <v>18</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18" s="5" t="s">
+      <c r="F18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -998,22 +989,22 @@
       <c r="C19" s="4">
         <v>14</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="5" t="s">
+      <c r="F19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1024,7 +1015,7 @@
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="4">
@@ -1033,16 +1024,16 @@
       <c r="E20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="5" t="s">
+      <c r="F20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1053,10 +1044,10 @@
       <c r="B21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1091,16 +1082,16 @@
       <c r="E22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I22" s="5" t="s">
+      <c r="F22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1178,16 +1169,16 @@
       <c r="E25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I25" s="5" t="s">
+      <c r="F25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1468,10 +1459,10 @@
       <c r="E35" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="5" t="s">
+      <c r="F35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H35" s="4">
@@ -1636,7 +1627,7 @@
       <c r="C41" s="4">
         <v>10</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -1723,7 +1714,7 @@
       <c r="C44" s="4">
         <v>16</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -1752,7 +1743,7 @@
       <c r="C45" s="4">
         <v>19</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -1810,7 +1801,7 @@
       <c r="C47" s="4">
         <v>3</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -1897,7 +1888,7 @@
       <c r="C50" s="4">
         <v>14</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -2013,7 +2004,7 @@
       <c r="C54" s="4">
         <v>8</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E54" s="3" t="s">
@@ -2303,7 +2294,7 @@
       <c r="C64" s="4">
         <v>32</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E64" s="3" t="s">
@@ -2332,7 +2323,7 @@
       <c r="C65" s="4">
         <v>5</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -2535,7 +2526,7 @@
       <c r="C72" s="4">
         <v>20</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E72" s="3" t="s">
@@ -2622,22 +2613,22 @@
       <c r="C75" s="4">
         <v>20</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F75" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I75" s="5" t="s">
+      <c r="F75" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I75" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2648,25 +2639,25 @@
       <c r="B76" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D76" s="5" t="s">
+      <c r="C76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F76" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I76" s="5" t="s">
+      <c r="F76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I76" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2686,16 +2677,16 @@
       <c r="E77" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F77" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I77" s="5" t="s">
+      <c r="F77" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I77" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2767,7 +2758,7 @@
       <c r="C80" s="4">
         <v>16</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E80" s="3" t="s">
@@ -2802,16 +2793,16 @@
       <c r="E81" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F81" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H81" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I81" s="5" t="s">
+      <c r="F81" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I81" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2854,7 +2845,7 @@
       <c r="C83" s="4">
         <v>14</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E83" s="3" t="s">
@@ -2883,7 +2874,7 @@
       <c r="C84" s="4">
         <v>6</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E84" s="3" t="s">
@@ -2912,7 +2903,7 @@
       <c r="C85" s="4">
         <v>20</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E85" s="3" t="s">
@@ -2979,7 +2970,7 @@
       <c r="F87" s="4">
         <v>5</v>
       </c>
-      <c r="G87" s="5" t="s">
+      <c r="G87" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H87" s="4">
@@ -2999,7 +2990,7 @@
       <c r="C88" s="4">
         <v>25</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E88" s="3" t="s">
@@ -3086,7 +3077,7 @@
       <c r="C91" s="4">
         <v>18</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E91" s="3" t="s">
@@ -3124,13 +3115,13 @@
       <c r="F92" s="4">
         <v>5</v>
       </c>
-      <c r="G92" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H92" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I92" s="5" t="s">
+      <c r="G92" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I92" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3228,7 +3219,7 @@
       <c r="B96" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C96" s="5" t="s">
+      <c r="C96" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D96" s="4">
@@ -3260,7 +3251,7 @@
       <c r="C97" s="4">
         <v>14</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E97" s="3" t="s">
@@ -3295,7 +3286,7 @@
       <c r="E98" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F98" s="5" t="s">
+      <c r="F98" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G98" s="4">
@@ -3318,7 +3309,7 @@
       <c r="C99" s="4">
         <v>15</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E99" s="3" t="s">
@@ -3405,22 +3396,22 @@
       <c r="C102" s="4">
         <v>1</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F102" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G102" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H102" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I102" s="5" t="s">
+      <c r="F102" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I102" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3434,7 +3425,7 @@
       <c r="C103" s="4">
         <v>16</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E103" s="3" t="s">
@@ -3469,16 +3460,16 @@
       <c r="E104" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F104" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G104" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H104" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I104" s="5" t="s">
+      <c r="F104" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I104" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3492,7 +3483,7 @@
       <c r="C105" s="4">
         <v>10</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="D105" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E105" s="3" t="s">
@@ -3579,7 +3570,7 @@
       <c r="C108" s="4">
         <v>10</v>
       </c>
-      <c r="D108" s="5" t="s">
+      <c r="D108" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E108" s="3" t="s">
@@ -3608,7 +3599,7 @@
       <c r="C109" s="4">
         <v>12</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="D109" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E109" s="3" t="s">
@@ -3666,16 +3657,16 @@
       <c r="C111" s="4">
         <v>15</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="D111" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F111" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G111" s="5" t="s">
+      <c r="F111" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H111" s="4">
@@ -3730,16 +3721,16 @@
       <c r="E113" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F113" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G113" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H113" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I113" s="5" t="s">
+      <c r="F113" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G113" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H113" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I113" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3750,25 +3741,25 @@
       <c r="B114" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C114" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D114" s="5" t="s">
+      <c r="C114" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F114" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G114" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H114" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I114" s="5" t="s">
+      <c r="F114" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H114" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I114" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3808,10 +3799,10 @@
       <c r="B116" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C116" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D116" s="5" t="s">
+      <c r="C116" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D116" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E116" s="3" t="s">
@@ -3869,7 +3860,7 @@
       <c r="C118" s="4">
         <v>14</v>
       </c>
-      <c r="D118" s="5" t="s">
+      <c r="D118" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E118" s="3" t="s">

</xml_diff>